<commit_message>
simulation and classes programmed and modified
</commit_message>
<xml_diff>
--- a/Dokumentation/Virus2SpreadClasses.xlsx
+++ b/Dokumentation/Virus2SpreadClasses.xlsx
@@ -34,7 +34,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Age = number of iterations. 
+          <t xml:space="preserve">age = number of iterations. 
 1 iteration = 1 day</t>
         </r>
       </text>
@@ -48,9 +48,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Rporduction Rate of a virus. 
-No values known, therefore a purely fictitious figure.
-The age  of a virus particel counted in Days</t>
+          <t xml:space="preserve">reporduction rate of a virus
+no values known, therefore a purely fictitious figure to play with 
+the age  of a virus particel counted in days
+1day = 1 iterateion</t>
         </r>
       </text>
     </comment>
@@ -63,9 +64,9 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">A virus is considered brocken "dead", when it can no longer replicate.
-No values known, therefore a purely fictitious number. 
-Age is counted in days, wehre 1 day is one iteration</t>
+          <t xml:space="preserve">a virus is considered brocken "dead", if it can no longer replicate
+no values known, therefore a purely fictitious number to play around 
+age is counted in days, wehre 1 day = 1 iteration</t>
         </r>
       </text>
     </comment>
@@ -78,7 +79,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Represents the status of a virus in its respective environment</t>
+          <t xml:space="preserve">represents the actual status of a virus in its respective environment</t>
         </r>
       </text>
     </comment>
@@ -91,7 +92,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The virus is brocken “dead” can no longer replicate or infect</t>
+          <t xml:space="preserve">the virus is brocken “dead” 
+can no longer replicate or infect people</t>
         </r>
       </text>
     </comment>
@@ -104,9 +106,9 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Saves Cell population density. 
-Determines the color shade of the grid cell 
-Higher with viruses populated Cells are brigther</t>
+          <t xml:space="preserve">saves CellPopulation density 
+determines the color shade of the grid cell 
+cells with higher viruses population are drawn brigther</t>
         </r>
       </text>
     </comment>
@@ -119,9 +121,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Object to pass the requiered
-MoveData 
-off the creature to the grid</t>
+          <t xml:space="preserve">helper object passes the requiered MoveData 
+from the creature to the grid</t>
         </r>
       </text>
     </comment>
@@ -134,8 +135,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">If virus state Reproducing create a new virus on a random grid cell.
-Depending on VirusReproductionRateByAge
+          <t xml:space="preserve">if virus state is Reproducing create a new virus on a random grid cell
+depending on VirusReproductionRateByAge
 </t>
         </r>
       </text>
@@ -149,7 +150,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Move over a random distance and direction, on random days.
+          <t xml:space="preserve">move over a random distance and direction, 
+on random days
 1 Iteration =  1day 
 depending on:
 MoveDistanceProfile
@@ -158,17 +160,16 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Age = number of iterations.
-1 iteration = 1 day</t>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">list of viruses</t>
         </r>
       </text>
     </comment>
@@ -181,15 +182,44 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The age-specific fertility rate (ASFR) 
-As numbers scaled out of 1000, i.e., the number of live births per 1000 women of a given age.
+          <t xml:space="preserve">create start configuration for the  InitialVirusPopulation number
+add the viruses on random grid cells 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">age = number of iterations
+1 iteration = 1 day = 1/364 years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">the age-specific fertility rate (ASFR) 
+as numbers scaled out of 1000, i.e., the number of live births per 1000 women of a given age.
 365 Iterations =
 1 year
 assumption 50% of population male/female</t>
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0">
+    <comment ref="A22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -199,78 +229,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">probability of death per 100000 people for a person’s age group.
-If 0.5 half of 100000 people of the randomly choosed person’s in this age group die.
-365 Iterations =
-1 year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Represents the states of a porson in its respective environment</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Person died</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">First Initial random start coordinate on the grid filed.
-Saved to move back home, like real persons do</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A21" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Saves Cell population density. 
-Determines the color shade of the grid cell
-Higher with person populated Cells are brigther</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Object pass the requiered MoveData 
-from creature to the grid</t>
+if 0.5 half of 100000 people of the randomly choosed person’s in this age group die.
+365 Iterations =1 year</t>
         </r>
       </text>
     </comment>
@@ -283,8 +243,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Create a new child person on a random grid cell. 
-Depending on PersonBirthRateByAge</t>
+          <t xml:space="preserve">represents the states of a porson in its respective environment</t>
         </r>
       </text>
     </comment>
@@ -297,7 +256,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">If Person State is Contagious, creates a new cirus on the actual GridCell</t>
+          <t xml:space="preserve">person died</t>
         </r>
       </text>
     </comment>
@@ -310,34 +269,189 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Move over a random distance and direction, on random days to new grid cell
+          <t xml:space="preserve">first initial random start coordinate on the grid filed.
+saved to move back home, 
+like most real persons do</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">saves population density of a grid cell 
+determines the color shade of that grid cell
+cells with higher person populations are brigther</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">helper object 
+passes the requiered MoveData 
+of a person/virus to the grid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">create a new child person on a random grid cell 
+depending on PersonBirthRateByAge</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">if PersonState is contagious, creates a new virus on the actual grid cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">move a random distance and direction, on random days to a new grid cell
 1 Iteration =  1day 
 depending on:
 MoveDistanceProfile
 MoveActivityRandom
-Remove form old grid coordinate, add to the new grid coordinate.
-get the CellPopulation from grid cell</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A26" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Move back to the home coordinate.
-To simulate working or travel traffic.
-Remove form old grid coordinate, add to the new grid coordinate.
-get the CellPopulation from grid cell
+adds a person to the new grid coordinate.
+and removes it from the old coordinate.
+get the CellPopulation from the new grid cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">move back to home coordinate
+to simulate working or travel traffic
+add the person to the home grid coordinate.
+remove person form the old grid coordinate.
+get the CellPopulation from the home grid cell
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0">
+    <comment ref="A34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">list of persons</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">create start configuration for the  InitialPersonPopulation number
+add the persons on random grid cells 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">object passes the requiered MoveData 
+from the creature to the grid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">current coordinate on the grid filed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">new coordiante on the grid field to move to</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">type of the creature virus or person</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -351,33 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Current coordinate on the grid filed</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">New grid field coordiante to move to</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A31" authorId="0">
+    <comment ref="B43" authorId="0">
       <text>
         <r>
           <rPr>
@@ -390,33 +478,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Object pass the requiered MoveData 
-from creature to the grid</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B31" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Type of creature virsu or person</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C1" authorId="0">
       <text>
         <r>
@@ -426,7 +487,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Represents actual states of the virus</t>
+          <t xml:space="preserve">represents actual state of the virus</t>
         </r>
       </text>
     </comment>
@@ -440,11 +501,12 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">motion profile
-Used to choose one from 10 distance ranges.
-Then calculate a random distance in choosed range.
-Get Random Direction 365° 
-To return relative moving vector (of type point)
-To simulate rare long distance moves.</t>
+used simulate moving behavior.
+chooses one from 10 distance ranges
+calculate a random distance in choosed range
+get random direction 365° 
+returns the new grid coordinate to move (of type point)
+</t>
         </r>
       </text>
     </comment>
@@ -458,11 +520,12 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">motion profile
-Used to choose one from 10 distance ranges.
-Then calculate a random distance in choosed range.
-Get Random Direction 365° 
-To return relative moving vector (of type point)
-To simulate rare long distance moves.</t>
+used to to simulate moving behavior
+choose one from 10 distance ranges
+calculate a random distance in choosed range
+get random direction 0-365° 
+return new grid cordinate to move (of type point)
+</t>
         </r>
       </text>
     </comment>
@@ -510,9 +573,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Random 
-get one move distance, fom the MoveDistnace 
-array</t>
+          <t xml:space="preserve">random get one of the 10 move distance ranges, fom the MoveDistnace array</t>
         </r>
       </text>
     </comment>
@@ -525,72 +586,72 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Returns a random new grid coordinate depending on the profile. 
-determines the new coordinate to move.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Represent actual  states of the person</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C17" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">How often the person was reinfected after recovering</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">motion profile
-Is used to simulate frequent short and rare long distance moves of people
-______________
-choose one from 10 distance ranges.
-get a random distance in the choosed range.
+          <t xml:space="preserve">returns a random new grid coordinate depending on the move profile. 
+determines the new coordinate to move</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">represent actual  states of the person</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">how often the person was reinfected after recovering</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">motion profile 
+used to simulate frequent short and rare long distance moves of people
+random choose one from 10 distance ranges
+get a random distance within the selected distance range
 get a random direction 365° 
-returns the NewGridCoordinattfor the move.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Holds 10 distnace ranges, to randomly choose one of them when moving
-Can be used to simulate rear far and frequent low distance moves of persons
+return the NewGridCoordinate for the move</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">holds 10 distnace ranges, 
+to randomly choose one of them when moving
+can be used to simulate tavle behavior rear far and frequent low distance moves of persons
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C25" authorId="0">
+    <comment ref="C30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -625,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C26" authorId="0">
+    <comment ref="C31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -635,7 +696,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">0 to 100 % 
-100% = move back home average every Iteration (day) 
+100% = move back home average every iteration (day) 
 50% = move back home averag evry 2</t>
         </r>
         <r>
@@ -655,36 +716,34 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve"> Iteration (day) 
+          <t xml:space="preserve"> iteration (day) 
 0% don’t move back home</t>
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Random 
-get one move distance, fom the MoveDistnace 
-array</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C28" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Returns a random new grid coordinate depending on the profile.
+    <comment ref="C32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">random get one move distance, fom the MoveDistnace array</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">returns a random new grid coordinate depending on the profile.
 determines the new coordinate to move.</t>
         </r>
       </text>
@@ -738,7 +797,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">High of the grid field</t>
+          <t xml:space="preserve">high of the grid field</t>
         </r>
       </text>
     </comment>
@@ -751,7 +810,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">A two dimensional array of GridCell objects</t>
+          <t xml:space="preserve">a two dimensional array of GridCell objects</t>
         </r>
       </text>
     </comment>
@@ -764,22 +823,22 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Add a person or virus to a grid cell on the grid field
-return the cell population. 
-(The number persons and number viruses a single cell contains)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I37" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Class used for ColorList</t>
+          <t xml:space="preserve">add a person/virus to a grid cell on the grid field
+delete it from the old field
+return the cell population (number persons and viruses on a the same grid cell coordinate)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">helper Class used for ColorList</t>
         </r>
       </text>
     </comment>
@@ -818,9 +877,9 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Cell population density. 
-Determines the color shade of the grid cell.
-Higer populated Cells are brigther</t>
+          <t xml:space="preserve">cell population density
+determines the color shade of a grid cell.
+higer populated cells are drawn brigther</t>
         </r>
       </text>
     </comment>
@@ -833,7 +892,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Helper Methods
+          <t xml:space="preserve">helper methods
 draw cell in differnet color shades for different population density</t>
         </r>
       </text>
@@ -847,7 +906,9 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Color of the grid cell depending on CellState</t>
+          <t xml:space="preserve">color of the grid cell depending on the CellState
+for example persons green, persons infected blue, viruses red 
+if the cell contains viruses and persons it is shown as infected person (blue)</t>
         </r>
       </text>
     </comment>
@@ -860,9 +921,9 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Cell population density. 
-Determines the color shade of the grid cell.
-Higer populated Cells are brigther</t>
+          <t xml:space="preserve">cell population density 
+determines the color shade of the grid cell
+higer populated Cells are drawn brigther</t>
         </r>
       </text>
     </comment>
@@ -889,9 +950,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Cell population density. 
-Determines the color shade of the grid cell.
-Higer populated Cells are brigther</t>
+          <t xml:space="preserve">number of persons and viruses on the same grid zell coordinate. 
+cell population density
+determines the color shade of the grid cell
+higer populated Cells are brigther</t>
         </r>
       </text>
     </comment>
@@ -900,7 +962,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
   <si>
     <t xml:space="preserve">Virus</t>
   </si>
@@ -1013,7 +1075,7 @@
     <t xml:space="preserve">PersAgeGroupsYear</t>
   </si>
   <si>
-    <t xml:space="preserve">MoveToData</t>
+    <t xml:space="preserve">VirMoveData</t>
   </si>
   <si>
     <t xml:space="preserve">MoveData</t>
@@ -1034,7 +1096,7 @@
     <t xml:space="preserve">()</t>
   </si>
   <si>
-    <t xml:space="preserve">GetNewCoordianteMoveTo</t>
+    <t xml:space="preserve">GetNewCoordianteToMove</t>
   </si>
   <si>
     <t xml:space="preserve">()Point</t>
@@ -1057,7 +1119,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(</t>
+      <t xml:space="preserve">(Grid) ret </t>
     </r>
     <r>
       <rPr>
@@ -1069,16 +1131,6 @@
       </rPr>
       <t xml:space="preserve">CellPopulation</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF111111"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">PersonInfected</t>
@@ -1099,6 +1151,33 @@
     <t xml:space="preserve">50-59</t>
   </si>
   <si>
+    <t xml:space="preserve">VirusList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60-69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viruses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List&lt;Virus&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70-79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SetInitialPopulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(long, Grid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100-119</t>
+  </si>
+  <si>
     <t xml:space="preserve">PersonState</t>
   </si>
   <si>
@@ -1108,25 +1187,19 @@
     <t xml:space="preserve">age in years</t>
   </si>
   <si>
-    <t xml:space="preserve">60-69</t>
-  </si>
-  <si>
     <t xml:space="preserve">Healthy</t>
   </si>
   <si>
     <t xml:space="preserve">GetBirthRateByAge</t>
   </si>
   <si>
-    <t xml:space="preserve">70-79</t>
-  </si>
-  <si>
     <t xml:space="preserve">PersonBirthRateByAge</t>
   </si>
   <si>
     <t xml:space="preserve">Infected</t>
   </si>
   <si>
-    <t xml:space="preserve">90-99</t>
+    <t xml:space="preserve">A Grid Cell (X,Y coordinat)” can contain multiple peron’s or viruses ,</t>
   </si>
   <si>
     <t xml:space="preserve">PersonDeathProbabilityByAge</t>
@@ -1135,7 +1208,7 @@
     <t xml:space="preserve">ReInfectionCounter</t>
   </si>
   <si>
-    <t xml:space="preserve">100-119</t>
+    <t xml:space="preserve">as they move random to new cell-coordinate, without a collision check.</t>
   </si>
   <si>
     <t xml:space="preserve">Contagious</t>
@@ -1150,6 +1223,12 @@
     <t xml:space="preserve">PersDeathRateByAgeGroup</t>
   </si>
   <si>
+    <t xml:space="preserve">Grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GridCell</t>
+  </si>
+  <si>
     <t xml:space="preserve">HomeCoordinate</t>
   </si>
   <si>
@@ -1159,82 +1238,58 @@
     <t xml:space="preserve">GetDeathRateByAge</t>
   </si>
   <si>
+    <t xml:space="preserve">maxX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PixelColor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumPersons</t>
+  </si>
+  <si>
     <t xml:space="preserve">GiveBirht</t>
   </si>
   <si>
-    <t xml:space="preserve">A Grid Cell (X,Y coordinat)” can contain multiple peron’s or viruses ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">as they move random to new cell-coordinate, without a collision check.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Childbirth</t>
+    <t xml:space="preserve">maxY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumViruses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersMoveData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gridField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GridCell[,] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChildBirth</t>
   </si>
   <si>
     <t xml:space="preserve">PersMoveDistanceProfile</t>
   </si>
   <si>
+    <t xml:space="preserve">SetNewEmptyGrid</t>
+  </si>
+  <si>
     <t xml:space="preserve">SpreadVirus</t>
   </si>
   <si>
     <t xml:space="preserve">PersonMoveDistance</t>
   </si>
   <si>
-    <t xml:space="preserve">Grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GridCell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PixelColor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumPersons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MoveToHomeCoordinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MoveHomeActivityRnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumViruses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GridCell[,] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GetNewMoveToCoordinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SetNewEmptyGrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OldGridCoordinate</t>
-  </si>
-  <si>
     <t xml:space="preserve">RemoveCreature</t>
   </si>
   <si>
     <t xml:space="preserve">(MoveData)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NewGridCoordinate</t>
   </si>
   <si>
     <t xml:space="preserve">AddCreature</t>
@@ -1265,6 +1320,12 @@
     <t xml:space="preserve">ColorExtensions</t>
   </si>
   <si>
+    <t xml:space="preserve">MoveToHomeCoordinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoveHomeActivityRnd</t>
+  </si>
+  <si>
     <t xml:space="preserve">ReturnMaxX</t>
   </si>
   <si>
@@ -1283,22 +1344,37 @@
     <t xml:space="preserve">(System.Drawing.Color) ret SixLabors.ImageSharp.Color</t>
   </si>
   <si>
+    <t xml:space="preserve">GetNewCoordinateToMove</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lighten</t>
   </si>
   <si>
     <t xml:space="preserve">(Color, double)</t>
   </si>
   <si>
+    <t xml:space="preserve">PersonList</t>
+  </si>
+  <si>
     <t xml:space="preserve">Darken</t>
   </si>
   <si>
+    <t xml:space="preserve">Persons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List&lt;Person&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ColorTranlation</t>
   </si>
   <si>
+    <t xml:space="preserve">CellStatus</t>
+  </si>
+  <si>
     <t xml:space="preserve">ColorList</t>
   </si>
   <si>
-    <t xml:space="preserve">CellStatus</t>
+    <t xml:space="preserve">CellColor</t>
   </si>
   <si>
     <t xml:space="preserve">colorList</t>
@@ -1307,10 +1383,13 @@
     <t xml:space="preserve">List&lt;ColorTranlation&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">CellColor</t>
-  </si>
-  <si>
     <t xml:space="preserve">GetColor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OldGridCoordinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NewGridCoordinate</t>
   </si>
 </sst>
 </file>
@@ -1360,14 +1439,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF3465A4"/>
+      <color rgb="FF729FCF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF3465A4"/>
+      <color rgb="FF729FCF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1438,16 +1517,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF8D1D75"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF8D1D75"/>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1460,8 +1531,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9.5"/>
-      <color rgb="FF000000"/>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF8D1D75"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8D1D75"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1624,7 +1703,7 @@
       <rgbColor rgb="FF158466"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FFA1467E"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -1654,7 +1733,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF972F"/>
       <rgbColor rgb="FFFF8000"/>
-      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -1673,16 +1752,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>55080</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>498240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>538920</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>765360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1695,8 +1774,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4937040" y="5047920"/>
-          <a:ext cx="3519720" cy="1329840"/>
+          <a:off x="17537760" y="0"/>
+          <a:ext cx="3518280" cy="1328400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1716,25 +1795,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="26.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.99"/>
@@ -1796,6 +1875,7 @@
       <c r="K2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="L2" s="5"/>
       <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1820,9 +1900,11 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="L3" s="5"/>
       <c r="N3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1935,6 +2017,7 @@
       <c r="K8" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
@@ -1952,9 +2035,11 @@
       <c r="I9" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
@@ -1967,155 +2052,106 @@
       <c r="I10" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="J10" s="5"/>
       <c r="K10" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3"/>
       <c r="I11" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
         <v>53</v>
       </c>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="12"/>
       <c r="K12" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K13" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="F14" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="5" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="D19" s="9"/>
+      <c r="F19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>13</v>
@@ -2123,63 +2159,77 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>38</v>
+        <v>17</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="I22" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
+      <c r="D24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="13" t="s">
+      <c r="G24" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L24" s="15"/>
       <c r="N24" s="14" t="s">
@@ -2188,14 +2238,23 @@
       <c r="O24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>49</v>
+      <c r="A25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>33</v>
+        <v>18</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>85</v>
@@ -2217,43 +2276,43 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="15" t="s">
         <v>90</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="J26" s="15" t="s">
         <v>9</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L26" s="15" t="s">
         <v>32</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O26" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>40</v>
+      <c r="A27" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>94</v>
@@ -2264,141 +2323,219 @@
       <c r="N27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="1" t="s">
+      <c r="A28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="B28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="9"/>
       <c r="I28" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>74</v>
+      <c r="A29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="18"/>
+      <c r="A30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="I30" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>4</v>
+      <c r="A31" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="19" t="s">
-        <v>106</v>
+      <c r="K31" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="I32" s="7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="19" t="s">
-        <v>109</v>
+      <c r="K32" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="K33" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="K34" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="17"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I37" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J37" s="15"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="I37" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="K37" s="14" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="L37" s="14"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I38" s="15" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="L38" s="15" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I39" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="K39" s="7" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="L39" s="7" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="19"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set grid cell color and population
</commit_message>
<xml_diff>
--- a/Dokumentation/Virus2SpreadClasses.xlsx
+++ b/Dokumentation/Virus2SpreadClasses.xlsx
@@ -842,6 +842,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="I42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">evaluate new CellPopulation depending on Creature Type
+evaluete CellState depending on cell population
+evaluate cell color depending on CelState
+set new GridCell, PixelColor and </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">CellPopulation</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> at the new creature coordinate.
+return new CellPopulation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K1" authorId="0">
       <text>
         <r>
@@ -962,7 +996,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="133">
   <si>
     <t xml:space="preserve">Virus</t>
   </si>
@@ -1391,6 +1425,15 @@
   <si>
     <t xml:space="preserve">NewGridCoordinate</t>
   </si>
+  <si>
+    <t xml:space="preserve">SetNewCellState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SetNewState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(MoveData , Grid) ret CellPopulation</t>
+  </si>
 </sst>
 </file>
 
@@ -1399,7 +1442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1551,6 +1594,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1759,9 +1807,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>765360</xdr:colOff>
+      <xdr:colOff>765000</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1775,7 +1823,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17537760" y="0"/>
-          <a:ext cx="3518280" cy="1328400"/>
+          <a:ext cx="3517920" cy="1328040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1795,10 +1843,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2529,6 +2577,9 @@
       <c r="B42" s="19" t="s">
         <v>83</v>
       </c>
+      <c r="I42" s="14" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="19" t="s">
@@ -2537,6 +2588,16 @@
       <c r="B43" s="19" t="s">
         <v>4</v>
       </c>
+      <c r="I43" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Some major changes to the movement functions
</commit_message>
<xml_diff>
--- a/Dokumentation/Virus2SpreadClasses.xlsx
+++ b/Dokumentation/Virus2SpreadClasses.xlsx
@@ -119,6 +119,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">helper object:
 pass the requiered move data of virus to the grid 
@@ -130,6 +131,7 @@
             <color rgb="FF000000"/>
             <rFont val="Cascadia Mono"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">- OldGridCoordinate 
 - NewGridCoordinate 
@@ -320,6 +322,7 @@
             <color rgb="FF000000"/>
             <rFont val="Cascadia Mono"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">- OldGridCoordinate
 - NewGridCoordinate
@@ -443,7 +446,43 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">current coordinate on the grid filed</t>
+          <t xml:space="preserve">current start </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">coordinate of </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">virus or person on the grid filed
+startpoint of movment
+i</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">f </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">VirusMoveGlobal or PersonMoveGlobal from configuration is set to true</t>
         </r>
       </text>
     </comment>
@@ -454,13 +493,44 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">new coordiante on the grid field to move to</t>
+          </rPr>
+          <t xml:space="preserve">end coordinate of </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">virus or person on the grid field to move to</t>
         </r>
       </text>
     </comment>
     <comment ref="A43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">home coordinate of virus or person on the grid filed
+used as always the same startpoint of movment 
+If </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">VirusMoveGlobal or PersonMoveGlobal from configuration is set to false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A44" authorId="0">
       <text>
         <r>
           <rPr>
@@ -487,7 +557,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0">
+    <comment ref="B44" authorId="0">
       <text>
         <r>
           <rPr>
@@ -777,18 +847,10 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Does the work to simulate activities
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">runs the iteration steps
+runs the iteration steps
 →  like person/virus moving, 
 by adding them to a new grid cell, and remove from old cell.
 → birth
@@ -1086,7 +1148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="156">
   <si>
     <t xml:space="preserve">Virus</t>
   </si>
@@ -1136,6 +1198,35 @@
     <t xml:space="preserve">GridMaxX</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Width of the Grid Filed - pixel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">VirusReproduceRateByAge</t>
   </si>
   <si>
@@ -1154,6 +1245,35 @@
     <t xml:space="preserve">GridMaxY</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Higth of the Grid Filed - pixel"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">VirusBrokenRateByAge</t>
   </si>
   <si>
@@ -1163,12 +1283,70 @@
     <t xml:space="preserve">long</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Start poulation for Viruses - long"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">VirMoveDistanceProfile</t>
   </si>
   <si>
     <t xml:space="preserve">InitialPersonPopulation</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Start poulation for Persons - long"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">IsBroken</t>
   </si>
   <si>
@@ -1181,6 +1359,38 @@
     <t xml:space="preserve">VirBrokenRateByAgeGroup</t>
   </si>
   <si>
+    <t xml:space="preserve">maxIterations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Number of maximal iterations for the Simulation - long"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">GridCellPopulation</t>
   </si>
   <si>
@@ -1199,6 +1409,38 @@
     <t xml:space="preserve">PersAgeGroupsYear</t>
   </si>
   <si>
+    <t xml:space="preserve">ColorList</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Not implemented yet - choose Grid Cell Colors"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">VirMoveData</t>
   </si>
   <si>
@@ -1214,13 +1456,45 @@
     <t xml:space="preserve">1-9</t>
   </si>
   <si>
+    <t xml:space="preserve">VirusMoveGlobal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"allow virus global moovment - true : movement within the distance limit only from the home coordinate. false: movement within the distance limit from the new current coordinate, therefore over the entire grid field possible"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Reproduce</t>
   </si>
   <si>
     <t xml:space="preserve">()</t>
   </si>
   <si>
-    <t xml:space="preserve">GetNewCoordianteToMove</t>
+    <t xml:space="preserve">GetEndCoordianteToMove</t>
   </si>
   <si>
     <t xml:space="preserve">()Point</t>
@@ -1230,6 +1504,38 @@
   </si>
   <si>
     <t xml:space="preserve">10-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonMoveGlobal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"allow person global moovment - true : movement within the distance limit only from the home coordinate. false: movement within the distance limit from the new current coordinate, therefore over the entire grid field possible"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">MoveToNewCoordinate</t>
@@ -1263,10 +1569,74 @@
     <t xml:space="preserve">20-29</t>
   </si>
   <si>
+    <t xml:space="preserve">TrackMovment</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"default false: If true allows movement tracking over the whole time - all iterations, as the person or virus at the old grid coordinate are not deleted after movment"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">EmtyCell</t>
   </si>
   <si>
     <t xml:space="preserve">30-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GridFormTimer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[Description(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Timer in milli seconds : standard 1 ms - bigger values slows down the iterations and the redraw of grid field form"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">)]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">40-49</t>
@@ -1468,7 +1838,7 @@
     <t xml:space="preserve">(System.Drawing.Color) ret SixLabors.ImageSharp.Color</t>
   </si>
   <si>
-    <t xml:space="preserve">GetNewCoordinateToMove</t>
+    <t xml:space="preserve">GetEndCoordinateToMove</t>
   </si>
   <si>
     <t xml:space="preserve">Lighten</t>
@@ -1495,9 +1865,6 @@
     <t xml:space="preserve">CellStatus</t>
   </si>
   <si>
-    <t xml:space="preserve">ColorList</t>
-  </si>
-  <si>
     <t xml:space="preserve">CellColor</t>
   </si>
   <si>
@@ -1513,16 +1880,19 @@
     <t xml:space="preserve">Simulation</t>
   </si>
   <si>
-    <t xml:space="preserve">OldGridCoordinate</t>
+    <t xml:space="preserve">StartGridCoordinate</t>
   </si>
   <si>
     <t xml:space="preserve">Grid.Grid</t>
   </si>
   <si>
-    <t xml:space="preserve">NewGridCoordinate</t>
+    <t xml:space="preserve">EndGridCoordinate</t>
   </si>
   <si>
     <t xml:space="preserve">SetNewCellState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HomeGridCoordinate</t>
   </si>
   <si>
     <t xml:space="preserve">SetNewState</t>
@@ -1553,7 +1923,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1620,8 +1990,27 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Cascadia Mono"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FFA31515"/>
+      <name val="Cascadia Mono"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF158466"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1671,13 +2060,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFA1467E"/>
       <name val="Arial"/>
@@ -1715,10 +2097,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFA7074B"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Cascadia Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1726,10 +2109,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9.5"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Cascadia Mono"/>
-      <family val="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -1781,7 +2164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1814,15 +2197,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1830,8 +2209,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1842,8 +2221,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1858,11 +2237,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1871,6 +2254,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1887,7 +2274,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1937,7 +2324,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FFA31515"/>
       <rgbColor rgb="FF8D1D75"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -1946,57 +2333,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>764640</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17537760" y="0"/>
-          <a:ext cx="3517560" cy="1327680"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2080,49 +2425,58 @@
       <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="P2" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="9"/>
       <c r="I3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3" s="5"/>
       <c r="N3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="P3" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3"/>
       <c r="N4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,668 +2487,730 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="D5" s="10"/>
       <c r="N5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>24</v>
+      <c r="P5" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="L8" s="5"/>
+      <c r="N8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="L9" s="5"/>
+      <c r="N9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>49</v>
+        <v>60</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="C10" s="3"/>
       <c r="I10" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="L10" s="5"/>
+      <c r="N10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3"/>
       <c r="I11" s="5" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="L11" s="5"/>
+      <c r="N11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12"/>
+      <c r="B12" s="14"/>
       <c r="K12" s="5" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="L12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K13" s="5" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="L13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="L14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="L15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="L16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K17" s="5" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="L17" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="F19" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>67</v>
+      <c r="A19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="F19" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="A21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="14" t="s">
-        <v>72</v>
+      <c r="I21" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="A22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="14" t="s">
-        <v>75</v>
+      <c r="I22" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="A23" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C24" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="L24" s="15"/>
-      <c r="N24" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="O24" s="15"/>
+      <c r="F24" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="L24" s="17"/>
+      <c r="N24" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="O24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="A25" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="15" t="s">
+      <c r="I25" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="J25" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="N25" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="O25" s="15" t="s">
+      <c r="K25" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="O25" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="A26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" s="15" t="s">
+      <c r="I26" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="N26" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="O26" s="15" t="s">
+      <c r="K26" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="O26" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="N27" s="15"/>
+      <c r="A27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="I28" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="I28" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>102</v>
+        <v>53</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>105</v>
+        <v>119</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>17</v>
+        <v>122</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="16" t="s">
-        <v>109</v>
+      <c r="K31" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>40</v>
+      <c r="C32" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="16" t="s">
-        <v>112</v>
+      <c r="K32" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
-        <v>117</v>
+      <c r="A34" s="15" t="s">
+        <v>133</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="17"/>
+      <c r="A35" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="J36" s="15"/>
+      <c r="A36" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="I37" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="L37" s="14"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="I37" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I38" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="K38" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="L38" s="15" t="s">
-        <v>126</v>
+      <c r="I38" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="0"/>
       <c r="K39" s="7" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20" t="s">
-        <v>128</v>
+      <c r="A40" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="21"/>
+      <c r="C40" s="22" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>80</v>
+      <c r="A41" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>132</v>
+      <c r="A42" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="J43" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B44" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="J43" s="15" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D44" s="21" t="s">
+      <c r="C44" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="7" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="7" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="0" t="s">
-        <v>138</v>
+      <c r="C47" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="7" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2805,7 +3221,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
different health states implemented
different health states implemented
</commit_message>
<xml_diff>
--- a/Dokumentation/Virus2SpreadClasses.xlsx
+++ b/Dokumentation/Virus2SpreadClasses.xlsx
@@ -337,6 +337,56 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Period from infection until a person is contagious.
+Default 2 days (iterations)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Period during which a person is infectious.
+Default 9 days (iterations)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Period during which a person is immune after after the recovery. Default  5 Month = 155 day (Iterations)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Percentage of reinfections after the immunity phase following an illness</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">create a new child person on a random grid cell 
@@ -344,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0">
+    <comment ref="A33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A30" authorId="0">
+    <comment ref="A34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -377,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0">
+    <comment ref="A35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -395,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A34" authorId="0">
+    <comment ref="A39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -408,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0">
+    <comment ref="A41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -423,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A40" authorId="0">
+    <comment ref="A45" authorId="0">
       <text>
         <r>
           <rPr>
@@ -437,43 +487,18 @@
         </r>
       </text>
     </comment>
-    <comment ref="A41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">current start </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">coordinate of </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">virus or person on the grid filed
+    <comment ref="A46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">current start coordinate of virus or person on the grid filed
 startpoint of movment
-i</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">f </t>
+if </t>
         </r>
         <r>
           <rPr>
@@ -481,39 +506,33 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">VirusMoveGlobal or PersonMoveGlobal from configuration is set to true</t>
         </r>
       </text>
     </comment>
-    <comment ref="A42" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">end coordinate of </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">virus or person on the grid field to move to</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A43" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+    <comment ref="A47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">end coordinate of virus or person on the grid field to move to</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">home coordinate of virus or person on the grid filed
 used as always the same startpoint of movment 
@@ -525,12 +544,13 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">VirusMoveGlobal or PersonMoveGlobal from configuration is set to false</t>
         </r>
       </text>
     </comment>
-    <comment ref="A44" authorId="0">
+    <comment ref="A49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -557,7 +577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0">
+    <comment ref="B49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -696,19 +716,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">how often the person was reinfected after recovering</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C28" authorId="0">
       <text>
         <r>
@@ -840,7 +847,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C40" authorId="0">
+    <comment ref="C44" authorId="0">
       <text>
         <r>
           <rPr>
@@ -861,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C45" authorId="0">
+    <comment ref="C49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -874,7 +881,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="0">
+    <comment ref="C50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -889,7 +896,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C47" authorId="0">
+    <comment ref="C51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -902,7 +909,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C48" authorId="0">
+    <comment ref="C52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1148,12 +1155,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="159">
   <si>
     <t xml:space="preserve">Virus</t>
   </si>
   <si>
-    <t xml:space="preserve">VirusState</t>
+    <t xml:space="preserve">ReinfectionImmunity</t>
   </si>
   <si>
     <t xml:space="preserve">VirReproduceRateByAgeGroup</t>
@@ -1204,6 +1211,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1213,6 +1221,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Width of the Grid Filed - pixel"</t>
     </r>
@@ -1222,6 +1231,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1251,6 +1261,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1260,6 +1271,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Higth of the Grid Filed - pixel"</t>
     </r>
@@ -1269,6 +1281,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1289,6 +1302,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1298,6 +1312,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Start poulation for Viruses - long"</t>
     </r>
@@ -1307,9 +1322,13 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">VirusState</t>
   </si>
   <si>
     <t xml:space="preserve">VirMoveDistanceProfile</t>
@@ -1324,6 +1343,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1333,6 +1353,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Start poulation for Persons - long"</t>
     </r>
@@ -1342,6 +1363,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1368,6 +1390,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1377,6 +1400,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Number of maximal iterations for the Simulation - long"</t>
     </r>
@@ -1386,6 +1410,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1418,6 +1443,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1427,6 +1453,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Not implemented yet - choose Grid Cell Colors"</t>
     </r>
@@ -1436,6 +1463,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1465,6 +1493,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1474,6 +1503,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"allow virus global moovment - true : movement within the distance limit only from the home coordinate. false: movement within the distance limit from the new current coordinate, therefore over the entire grid field possible"</t>
     </r>
@@ -1483,6 +1513,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1515,6 +1546,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1524,6 +1556,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"allow person global moovment - true : movement within the distance limit only from the home coordinate. false: movement within the distance limit from the new current coordinate, therefore over the entire grid field possible"</t>
     </r>
@@ -1533,6 +1566,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1578,6 +1612,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1587,6 +1622,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"default false: If true allows movement tracking over the whole time - all iterations, as the person or virus at the old grid coordinate are not deleted after movment"</t>
     </r>
@@ -1596,6 +1632,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
@@ -1616,6 +1653,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[Description(</t>
     </r>
@@ -1625,6 +1663,7 @@
         <color rgb="FFA31515"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Timer in milli seconds : standard 1 ms - bigger values slows down the iterations and the redraw of grid field form"</t>
     </r>
@@ -1634,14 +1673,21 @@
         <color rgb="FF000000"/>
         <rFont val="Cascadia Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)]</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Contagious</t>
+  </si>
+  <si>
     <t xml:space="preserve">40-49</t>
   </si>
   <si>
+    <t xml:space="preserve">Recoverd</t>
+  </si>
+  <si>
     <t xml:space="preserve">50-59</t>
   </si>
   <si>
@@ -1681,16 +1727,13 @@
     <t xml:space="preserve">age in years</t>
   </si>
   <si>
-    <t xml:space="preserve">Healthy</t>
-  </si>
-  <si>
     <t xml:space="preserve">GetBirthRateByAge</t>
   </si>
   <si>
     <t xml:space="preserve">PersonBirthRateByAge</t>
   </si>
   <si>
-    <t xml:space="preserve">Infected</t>
+    <t xml:space="preserve">HealthStateCounter</t>
   </si>
   <si>
     <t xml:space="preserve">A Grid Cell (X,Y coordinat)” can contain multiple peron’s or viruses ,</t>
@@ -1699,21 +1742,12 @@
     <t xml:space="preserve">PersonDeathProbabilityByAge</t>
   </si>
   <si>
-    <t xml:space="preserve">ReInfectionCounter</t>
-  </si>
-  <si>
     <t xml:space="preserve">as they move random to new cell-coordinate, without a collision check.</t>
   </si>
   <si>
-    <t xml:space="preserve">Contagious</t>
-  </si>
-  <si>
     <t xml:space="preserve">IsDead</t>
   </si>
   <si>
-    <t xml:space="preserve">Recoverd</t>
-  </si>
-  <si>
     <t xml:space="preserve">PersDeathRateByAgeGroup</t>
   </si>
   <si>
@@ -1744,9 +1778,6 @@
     <t xml:space="preserve">NumPersons</t>
   </si>
   <si>
-    <t xml:space="preserve">GiveBirht</t>
-  </si>
-  <si>
     <t xml:space="preserve">maxY</t>
   </si>
   <si>
@@ -1765,7 +1796,7 @@
     <t xml:space="preserve">GridCell[,] </t>
   </si>
   <si>
-    <t xml:space="preserve">ChildBirth</t>
+    <t xml:space="preserve">PersonLatencyPeriod</t>
   </si>
   <si>
     <t xml:space="preserve">PersMoveDistanceProfile</t>
@@ -1774,7 +1805,7 @@
     <t xml:space="preserve">SetNewEmptyGrid</t>
   </si>
   <si>
-    <t xml:space="preserve">SpreadVirus</t>
+    <t xml:space="preserve">PersonInfectiousPeriod </t>
   </si>
   <si>
     <t xml:space="preserve">PersonMoveDistance</t>
@@ -1784,6 +1815,9 @@
   </si>
   <si>
     <t xml:space="preserve">(MoveData)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PersonReinfectionImmunityPeriod</t>
   </si>
   <si>
     <t xml:space="preserve">AddCreatureToCell</t>
@@ -1814,43 +1848,73 @@
     <t xml:space="preserve">ColorExtensions</t>
   </si>
   <si>
+    <t xml:space="preserve">PersonReinfectionRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoveHomeActivityRnd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReturnMaxX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ToSystemDrawingColor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(SixLabors.ImageSharp.Color) ret System.Drawing.Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChildBirth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReturnMaxY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ToImageSharpColor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(System.Drawing.Color) ret SixLabors.ImageSharp.Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpreadVirus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetEndCoordinateToMove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lighten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Color, double)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darken</t>
+  </si>
+  <si>
     <t xml:space="preserve">MoveToHomeCoordinate</t>
   </si>
   <si>
-    <t xml:space="preserve">MoveHomeActivityRnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReturnMaxX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ToSystemDrawingColor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(SixLabors.ImageSharp.Color) ret System.Drawing.Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReturnMaxY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ToImageSharpColor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(System.Drawing.Color) ret SixLabors.ImageSharp.Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GetEndCoordinateToMove</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lighten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Color, double)</t>
+    <t xml:space="preserve">ColorTranlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CellColor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colorList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List&lt;ColorTranlation&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">PersonList</t>
   </si>
   <si>
-    <t xml:space="preserve">Darken</t>
+    <t xml:space="preserve">GetColor</t>
   </si>
   <si>
     <t xml:space="preserve">Persons</t>
@@ -1859,46 +1923,28 @@
     <t xml:space="preserve">List&lt;Person&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">ColorTranlation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CellStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CellColor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">colorList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List&lt;ColorTranlation&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GetColor</t>
+    <t xml:space="preserve">SetNewCellState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SetNewState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(MoveData , Grid) ret CellPopulation</t>
   </si>
   <si>
     <t xml:space="preserve">Simulation</t>
   </si>
   <si>
+    <t xml:space="preserve">Grid.Grid</t>
+  </si>
+  <si>
     <t xml:space="preserve">StartGridCoordinate</t>
   </si>
   <si>
-    <t xml:space="preserve">Grid.Grid</t>
-  </si>
-  <si>
     <t xml:space="preserve">EndGridCoordinate</t>
   </si>
   <si>
-    <t xml:space="preserve">SetNewCellState</t>
-  </si>
-  <si>
     <t xml:space="preserve">HomeGridCoordinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SetNewState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(MoveData , Grid) ret CellPopulation</t>
   </si>
   <si>
     <t xml:space="preserve">iteration</t>
@@ -1923,7 +1969,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1961,6 +2007,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF158466"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF729FCF"/>
@@ -1994,12 +2046,14 @@
       <color rgb="FF000000"/>
       <name val="Cascadia Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9.5"/>
       <color rgb="FFA31515"/>
       <name val="Cascadia Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2068,6 +2122,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="9.5"/>
+      <color rgb="FFA7074B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF8D1D75"/>
       <name val="Arial"/>
@@ -2082,8 +2144,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="9.5"/>
+      <sz val="10"/>
       <color rgb="FFA7074B"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -2091,26 +2152,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFA7074B"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9.5"/>
-      <color rgb="FF000000"/>
-      <name val="Cascadia Mono"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2197,7 +2238,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2205,11 +2250,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2221,12 +2262,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2234,10 +2275,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2258,6 +2295,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2338,15 +2379,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.72"/>
@@ -2367,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -2376,19 +2417,19 @@
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2405,27 +2446,27 @@
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="5"/>
+      <c r="L2" s="6"/>
       <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2442,22 +2483,22 @@
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="I3" s="5" t="s">
+      <c r="G3" s="10"/>
+      <c r="I3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="6"/>
       <c r="N3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2475,540 +2516,522 @@
       <c r="O4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="D5" s="11"/>
       <c r="N5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="8" t="s">
-        <v>30</v>
+      <c r="P5" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="8" t="s">
-        <v>36</v>
+      <c r="P6" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="5" t="s">
+      <c r="K7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="8" t="s">
         <v>44</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="D8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="6"/>
       <c r="N8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="8" t="s">
-        <v>51</v>
+      <c r="P8" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>53</v>
       </c>
+      <c r="B9" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="6"/>
       <c r="N9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="8" t="s">
-        <v>59</v>
+      <c r="P9" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="B10" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="C10" s="3"/>
-      <c r="I10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="6"/>
       <c r="N10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P10" s="8" t="s">
-        <v>65</v>
+      <c r="P10" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3"/>
-      <c r="I11" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5" t="s">
+      <c r="I11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="6"/>
       <c r="N11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P11" s="8" t="s">
-        <v>69</v>
+      <c r="P11" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="14"/>
-      <c r="K12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" s="5"/>
+      <c r="B12" s="15"/>
+      <c r="I12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L13" s="5"/>
+      <c r="I13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L14" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="L15" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L16" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="L17" s="5"/>
+      <c r="K17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="F19" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>83</v>
+      <c r="B19" s="11"/>
+      <c r="C19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="F19" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="F20" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="11"/>
+      <c r="I22" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="B23" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="7" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="F24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="18"/>
+      <c r="K24" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" s="18"/>
+      <c r="N24" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="O24" s="18"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="F25" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="I25" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="O25" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="I26" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="O26" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="N27" s="18"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="I28" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="I31" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="L24" s="17"/>
-      <c r="N24" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="O24" s="17"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="N25" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="O25" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="L26" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N26" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="O26" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="N27" s="17"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="I28" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K31" s="18" t="s">
+      <c r="K31" s="12" t="s">
         <v>125</v>
       </c>
       <c r="L31" s="1" t="s">
@@ -3016,201 +3039,233 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="12" t="s">
+      <c r="A32" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36" s="18"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L37" s="17"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="L38" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="K39" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="I42" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I43" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J43" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="J32" s="7" t="s">
+      <c r="B45" s="22"/>
+      <c r="C45" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" s="19"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="J36" s="17"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="I37" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K37" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L37" s="16"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I38" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="L38" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K39" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="B43" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B49" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="7" t="s">
+      <c r="C49" s="8" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>